<commit_message>
Optimized Alot, Fixed TestNG.XML
</commit_message>
<xml_diff>
--- a/src/main/java/resources/TestData.xlsx
+++ b/src/main/java/resources/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Selenium\frameworkSelneiumBatch2-ChrisMensing\src\main\java\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christopher.mensing\Documents\Code\Java Programs\AutomationTrainingFinalProject\frameworkSelneiumBatch2\src\main\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB65F005-9B27-48B1-94BD-54EDD24B3748}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E249BC0-88EA-46C8-B443-350E77FBEFB1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4710" windowWidth="29040" windowHeight="16440" tabRatio="710" activeTab="3" xr2:uid="{3D83174F-648F-435E-BEBC-5633B04CF0E4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="710" activeTab="4" xr2:uid="{3D83174F-648F-435E-BEBC-5633B04CF0E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes About this Excel" sheetId="14" r:id="rId1"/>
@@ -25,17 +25,23 @@
   <definedNames>
     <definedName name="Broswers">BackEnd!$A$4:$A$8:INDEX(BackEnd!$A$4:$A$8,SUMPRODUCT(--(BackEnd!$A$4:$A$8&lt;&gt;"")))</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="127">
   <si>
     <t>Broswer</t>
   </si>
@@ -365,23 +371,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Additional Search Details
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note: Text Must Match, IE in software you can click on Download under software Delivery Method
-Note2: Separate the Terms By a  :</t>
-    </r>
-  </si>
-  <si>
     <t>All Sheets Must Not have Empty Cells, if there is an empty cell the row will be skipped in the data provider</t>
   </si>
   <si>
@@ -500,9 +489,6 @@
     <t>Master Selenium WebDriver Book</t>
   </si>
   <si>
-    <t>Paperback</t>
-  </si>
-  <si>
     <t>Expected Results</t>
   </si>
   <si>
@@ -558,6 +544,41 @@
   </si>
   <si>
     <t>No Product Results</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Additional Search Details
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: Text Must Match, IE in software you can click on Download under software Delivery Method
+Note2: Separate the Terms By a  :N:</t>
+    </r>
+  </si>
+  <si>
+    <t>Paperback:N:Used</t>
+  </si>
+  <si>
+    <t>Software Test Automation</t>
+  </si>
+  <si>
+    <t>Verify The Book QuickTest  Professional Unplugged is Present</t>
+  </si>
+  <si>
+    <t>QuickTest Professional Unplugged</t>
+  </si>
+  <si>
+    <t>img[alt='QuickTest Professional Unplugged']</t>
+  </si>
+  <si>
+    <t>img[alt='Software Test Automation']</t>
   </si>
 </sst>
 </file>
@@ -989,7 +1010,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -999,22 +1020,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1044,7 +1065,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1053,7 +1074,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1070,7 +1091,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1087,7 +1108,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -1104,7 +1125,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -1121,7 +1142,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -1199,7 +1220,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1208,15 +1229,15 @@
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1225,7 +1246,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -1233,7 +1254,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -1242,7 +1263,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
@@ -1277,10 +1298,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9481859A-3089-43B6-A834-0C76241877F0}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,7 +1330,7 @@
     </row>
     <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -1318,7 +1339,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -1333,7 +1354,7 @@
         <v>80</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="J2" t="s">
         <v>78</v>
@@ -1341,7 +1362,7 @@
     </row>
     <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>2</v>
@@ -1350,22 +1371,22 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E3" t="s">
         <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="J3" t="b">
         <v>0</v>
@@ -1373,7 +1394,7 @@
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>2</v>
@@ -1382,25 +1403,57 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E4" t="s">
         <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I4" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="J4" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1408,7 +1461,7 @@
     <mergeCell ref="D1:J1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G1048576 J3:J1048576" xr:uid="{7B640E7F-2BBA-473B-A0A5-4047A2B1B736}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J1048576 G3:G1048576" xr:uid="{7B640E7F-2BBA-473B-A0A5-4047A2B1B736}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576" xr:uid="{89918396-C10C-4F7D-838F-A9FB01B2740E}">
@@ -1434,10 +1487,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDDB5B45-EDFB-43F8-AD41-673A561A912A}">
-  <dimension ref="A2:K4"/>
+  <dimension ref="A2:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,82 +1509,104 @@
   <sheetData>
     <row r="2" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" t="s">
         <v>112</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>113</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>114</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>115</v>
-      </c>
-      <c r="J2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
       </c>
       <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1545,7 +1620,7 @@
           <x14:formula1>
             <xm:f>BackEnd!$A$10:$A$30</xm:f>
           </x14:formula1>
-          <xm:sqref>C4</xm:sqref>
+          <xm:sqref>C3:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1570,7 +1645,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1582,23 +1657,23 @@
     </row>
     <row r="2" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>